<commit_message>
Add PT100 REV D
</commit_message>
<xml_diff>
--- a/hw/Master BOM.xlsx
+++ b/hw/Master BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="248">
   <si>
     <t>Description</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Tensility</t>
   </si>
   <si>
-    <t>Hirose</t>
-  </si>
-  <si>
     <t>CONN PLUG MALE 6POS SOLDER CUP</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Analog Devices Inc.</t>
   </si>
   <si>
-    <t>OSH Park</t>
-  </si>
-  <si>
     <t>Designator</t>
   </si>
   <si>
@@ -317,9 +311,6 @@
     <t>Screw Hex Zinc Plt Steel, 6-32, 1/4 (1)</t>
   </si>
   <si>
-    <t>CABLE 6COND 28AWG BLK (0.5M)</t>
-  </si>
-  <si>
     <t>U3</t>
   </si>
   <si>
@@ -338,21 +329,6 @@
     <t>C13</t>
   </si>
   <si>
-    <t>C4, C5</t>
-  </si>
-  <si>
-    <t>C11, C12</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
-    <t>C14, C16</t>
-  </si>
-  <si>
     <t>C15</t>
   </si>
   <si>
@@ -362,15 +338,9 @@
     <t>C23</t>
   </si>
   <si>
-    <t>C2, C8, C19, C22</t>
-  </si>
-  <si>
     <t>R1</t>
   </si>
   <si>
-    <t>R2, R3</t>
-  </si>
-  <si>
     <t>R7</t>
   </si>
   <si>
@@ -383,15 +353,6 @@
     <t>R6</t>
   </si>
   <si>
-    <t>R8, R11, R15</t>
-  </si>
-  <si>
-    <t>R9, R12</t>
-  </si>
-  <si>
-    <t>R10, R13</t>
-  </si>
-  <si>
     <t>R14</t>
   </si>
   <si>
@@ -593,9 +554,6 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>FB2, FB3</t>
-  </si>
-  <si>
     <t>BK1608LM182-T</t>
   </si>
   <si>
@@ -683,9 +641,6 @@
     <t>AC101A</t>
   </si>
   <si>
-    <t>C1, C3, C6, C7, C9, C10, C18, C20, C21, C24</t>
-  </si>
-  <si>
     <t>LED1</t>
   </si>
   <si>
@@ -696,6 +651,123 @@
   </si>
   <si>
     <t>PT102 REV C</t>
+  </si>
+  <si>
+    <t>KFD100 1.1</t>
+  </si>
+  <si>
+    <t>PT100 REV D</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>TVS DIODE 5.25V 17V SOT23-6</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>497-5235-1-ND</t>
+  </si>
+  <si>
+    <t>511-USBLC6-2SC6</t>
+  </si>
+  <si>
+    <t>AC102A</t>
+  </si>
+  <si>
+    <t>HR10A-7J-6S(73)</t>
+  </si>
+  <si>
+    <t>CONN JACK FMALE 6POS SOLDER CUP</t>
+  </si>
+  <si>
+    <t>HR1601-ND</t>
+  </si>
+  <si>
+    <t>798-HR10A-7J-6S73</t>
+  </si>
+  <si>
+    <t>AC103A</t>
+  </si>
+  <si>
+    <t>Amphenol Sine Systems Corp</t>
+  </si>
+  <si>
+    <t>T3360018U</t>
+  </si>
+  <si>
+    <t>CONN PLUG MALE DIN 5POS SLDR CUP</t>
+  </si>
+  <si>
+    <t>361-1217-ND</t>
+  </si>
+  <si>
+    <t>AC104A</t>
+  </si>
+  <si>
+    <t>CONN MOD PLUG 8P8C UNSHIELDED</t>
+  </si>
+  <si>
+    <t>Stewart Connector</t>
+  </si>
+  <si>
+    <t>940-SP-3088</t>
+  </si>
+  <si>
+    <t>380-1192-ND</t>
+  </si>
+  <si>
+    <t>530-940-SP-3088</t>
+  </si>
+  <si>
+    <t>CABLE 6COND 28AWG BLK 153M (0.5M)</t>
+  </si>
+  <si>
+    <t>CABLE 6COND 28AWG BLK 153M (0.15M)</t>
+  </si>
+  <si>
+    <t>C4,C5</t>
+  </si>
+  <si>
+    <t>C11,C12</t>
+  </si>
+  <si>
+    <t>C1,C3,C6,C7,C9,C10,C18,C20,C21,C24</t>
+  </si>
+  <si>
+    <t>C14,C16</t>
+  </si>
+  <si>
+    <t>C2,C8,C19,C22</t>
+  </si>
+  <si>
+    <t>FB2,FB3</t>
+  </si>
+  <si>
+    <t>D1,D2</t>
+  </si>
+  <si>
+    <t>J2,J3</t>
+  </si>
+  <si>
+    <t>R2,R3</t>
+  </si>
+  <si>
+    <t>Q1,Q2</t>
+  </si>
+  <si>
+    <t>R10,R13</t>
+  </si>
+  <si>
+    <t>R9,R12</t>
+  </si>
+  <si>
+    <t>R8,R11,R15</t>
   </si>
 </sst>
 </file>
@@ -748,7 +820,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -770,15 +842,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1060,7 +1123,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I52"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:I110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1069,8 +1135,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1085,8 +1151,8 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>45</v>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>13</v>
@@ -1104,15 +1170,15 @@
         <v>7</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
-      <c r="B2" s="8"/>
+      <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="7"/>
@@ -1123,9 +1189,9 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="9"/>
+        <v>91</v>
+      </c>
+      <c r="B3" s="6"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
       <c r="E3" s="4"/>
@@ -1136,74 +1202,74 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="1">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>23</v>
+      <c r="B5" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>104</v>
+        <v>148</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -1212,27 +1278,27 @@
         <v>9</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>105</v>
+        <v>152</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -1241,27 +1307,27 @@
         <v>9</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>111</v>
+        <v>155</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="E8" s="1">
         <v>1</v>
@@ -1270,27 +1336,27 @@
         <v>9</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>103</v>
+        <v>156</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
@@ -1299,27 +1365,27 @@
         <v>9</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>219</v>
+        <v>159</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>173</v>
+        <v>160</v>
       </c>
       <c r="E10" s="1">
         <v>10</v>
@@ -1328,27 +1394,27 @@
         <v>9</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>162</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>176</v>
+        <v>163</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -1357,27 +1423,27 @@
         <v>9</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>109</v>
+        <v>165</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
@@ -1386,27 +1452,27 @@
         <v>9</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>110</v>
+        <v>168</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1415,27 +1481,27 @@
         <v>9</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>112</v>
+        <v>171</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>239</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="E14" s="1">
         <v>4</v>
@@ -1444,27 +1510,27 @@
         <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1473,56 +1539,56 @@
         <v>9</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E16" s="2">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>49</v>
+        <v>110</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="E17" s="1">
         <v>1</v>
@@ -1531,27 +1597,27 @@
         <v>9</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E18" s="1">
         <v>1</v>
@@ -1560,27 +1626,27 @@
         <v>9</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>189</v>
+        <v>174</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>240</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -1589,56 +1655,56 @@
         <v>9</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="2">
-        <v>1</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>217</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E21" s="2">
         <v>2</v>
@@ -1647,27 +1713,27 @@
         <v>9</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="E22" s="2">
         <v>2</v>
@@ -1676,27 +1742,27 @@
         <v>9</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>114</v>
+        <v>120</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E23" s="2">
         <v>2</v>
@@ -1705,27 +1771,27 @@
         <v>9</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>118</v>
+        <v>123</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -1734,27 +1800,27 @@
         <v>9</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>121</v>
+        <v>125</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>245</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E25" s="2">
         <v>2</v>
@@ -1763,27 +1829,27 @@
         <v>9</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>113</v>
+        <v>127</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -1792,27 +1858,27 @@
         <v>9</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>120</v>
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>246</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="E27" s="2">
         <v>2</v>
@@ -1821,27 +1887,27 @@
         <v>9</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B28" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D28" s="2" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -1850,27 +1916,27 @@
         <v>9</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>119</v>
+        <v>136</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>247</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E29" s="2">
         <v>3</v>
@@ -1879,27 +1945,27 @@
         <v>9</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>122</v>
+        <v>139</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>109</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E30" s="2">
         <v>1</v>
@@ -1908,27 +1974,27 @@
         <v>9</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>116</v>
+        <v>142</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="E31" s="2">
         <v>1</v>
@@ -1937,27 +2003,27 @@
         <v>9</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>115</v>
+        <v>145</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="E32" s="2">
         <v>1</v>
@@ -1966,85 +2032,85 @@
         <v>9</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="D33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="1">
-        <v>1</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="H34" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -2053,56 +2119,56 @@
         <v>9</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B36" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E36" s="1">
+        <v>1</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="H36" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="E36" s="1">
-        <v>1</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>197</v>
+        <v>186</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>183</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="E37" s="1">
         <v>1</v>
@@ -2111,169 +2177,169 @@
         <v>9</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38" s="2">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B39" s="10" t="s">
         <v>23</v>
       </c>
+      <c r="B39" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C39" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="E39" s="1">
         <v>1</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>23</v>
+        <v>94</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E40" s="1">
         <v>4</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>23</v>
+      <c r="B42" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E42" s="1">
         <v>1</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>2</v>
@@ -2288,24 +2354,24 @@
         <v>3</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>23</v>
+        <v>68</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E44" s="2">
         <v>2</v>
@@ -2314,26 +2380,23 @@
         <v>9</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E45" s="1"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="B46" s="9"/>
+        <v>209</v>
+      </c>
+      <c r="B46" s="6"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="E46" s="4"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -2341,135 +2404,1640 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>23</v>
+        <v>29</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E47" s="2">
+        <v>30</v>
+      </c>
+      <c r="E47" s="1">
         <v>1</v>
       </c>
       <c r="F47" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="2">
+        <v>210</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E49" s="1">
         <v>2</v>
       </c>
-      <c r="F48" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>81</v>
+      <c r="F49" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
+      <c r="A50" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>23</v>
+        <v>155</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>14</v>
+        <v>114</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E51" s="2">
+        <v>115</v>
+      </c>
+      <c r="E51" s="1">
         <v>1</v>
       </c>
       <c r="F51" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="I51" s="2" t="s">
-        <v>23</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E53" s="1">
+        <v>10</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E54" s="1">
+        <v>2</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E55" s="1">
+        <v>1</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E56" s="1">
+        <v>1</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" s="1">
+        <v>4</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E58" s="1">
+        <v>2</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E59" s="2">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E62" s="1">
+        <v>2</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="2">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64" s="2">
+        <v>2</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H64" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E65" s="2">
+        <v>2</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E66" s="2">
+        <v>2</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="H66" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E67" s="2">
+        <v>1</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I67" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E68" s="2">
+        <v>2</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E69" s="2">
+        <v>1</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E70" s="2">
+        <v>2</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E72" s="2">
+        <v>3</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E73" s="2">
+        <v>1</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H73" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E74" s="2">
+        <v>1</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E75" s="2">
+        <v>1</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" s="1">
+        <v>1</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I76" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H77" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I77" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E78" s="1">
+        <v>1</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H78" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I78" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E79" s="1">
+        <v>1</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H79" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E80" s="1">
+        <v>1</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E81" s="1">
+        <v>1</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E82" s="2">
+        <v>1</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G82" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I82" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="E83" s="1">
+        <v>1</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I83" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E84" s="1">
+        <v>4</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E85" s="1">
+        <v>1</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="1">
+        <v>1</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C52" s="2" t="s">
+      <c r="B87" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="2">
+        <v>1</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E88" s="2">
+        <v>2</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H88" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E89" s="1"/>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="3"/>
+      <c r="F90" s="3"/>
+      <c r="G90" s="3"/>
+      <c r="H90" s="3"/>
+      <c r="I90" s="3"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="2">
+        <v>1</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="2" t="s">
+      <c r="B92" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D92" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="2">
-        <v>1</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G52" s="2" t="s">
+      <c r="E92" s="2">
+        <v>2</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G92" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H52" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>81</v>
+      <c r="H92" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B94" s="6"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+      <c r="G94" s="3"/>
+      <c r="H94" s="3"/>
+      <c r="I94" s="3"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="2">
+        <v>1</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H95" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="2">
+        <v>1</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I96" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="B98" s="6"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3"/>
+      <c r="G98" s="3"/>
+      <c r="H98" s="3"/>
+      <c r="I98" s="3"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="2">
+        <v>1</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H99" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I99" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E100" s="2">
+        <v>1</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H100" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I100" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="B102" s="6"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3"/>
+      <c r="G102" s="3"/>
+      <c r="H102" s="3"/>
+      <c r="I102" s="3"/>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="2">
+        <v>1</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H103" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H104" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I104" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E105" s="2">
+        <v>1</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="B107" s="6"/>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3"/>
+      <c r="G107" s="3"/>
+      <c r="H107" s="3"/>
+      <c r="I107" s="3"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="2">
+        <v>1</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E110" s="2">
+        <v>1</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H110" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="0" scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
HW: Add AC104B, AC105A, AC106A to BOM
</commit_message>
<xml_diff>
--- a/hw/Master BOM.xlsx
+++ b/hw/Master BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="265">
   <si>
     <t>Description</t>
   </si>
@@ -768,6 +768,57 @@
   </si>
   <si>
     <t>R8,R11,R15</t>
+  </si>
+  <si>
+    <t>AC104B</t>
+  </si>
+  <si>
+    <t>AC105A</t>
+  </si>
+  <si>
+    <t>AC106A</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V SGL DO35</t>
+  </si>
+  <si>
+    <t>Vishay Semiconductor Diodes</t>
+  </si>
+  <si>
+    <t>SD103A-TAP</t>
+  </si>
+  <si>
+    <t>SD103A-TAPGICT-ND</t>
+  </si>
+  <si>
+    <t>78-SD103A-TAP</t>
+  </si>
+  <si>
+    <t>Kenwood Portable Accessory Connector</t>
+  </si>
+  <si>
+    <t>1551MBK</t>
+  </si>
+  <si>
+    <t>HM993-ND</t>
+  </si>
+  <si>
+    <t>BOX ABS BLACK 1.38"L X 1.38"W</t>
+  </si>
+  <si>
+    <t>546-1551MBK</t>
+  </si>
+  <si>
+    <t>CONN RCPT FMALE 6POS SOLDER CUP</t>
+  </si>
+  <si>
+    <t>HR10A-7R-6S(73)</t>
+  </si>
+  <si>
+    <t>HR1594-ND</t>
+  </si>
+  <si>
+    <t>798-HR10A-7R-6S73</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1177,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4036,6 +4087,335 @@
         <v>232</v>
       </c>
     </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B112" s="6"/>
+      <c r="C112" s="3"/>
+      <c r="D112" s="3"/>
+      <c r="E112" s="3"/>
+      <c r="F112" s="3"/>
+      <c r="G112" s="3"/>
+      <c r="H112" s="3"/>
+      <c r="I112" s="3"/>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113" s="2">
+        <v>1</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H113" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I113" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E114" s="2">
+        <v>1</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H114" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I114" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E115" s="2">
+        <v>1</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H115" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I115" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E116" s="2">
+        <v>1</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B118" s="6"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3"/>
+      <c r="G118" s="3"/>
+      <c r="H118" s="3"/>
+      <c r="I118" s="3"/>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E119" s="2">
+        <v>1</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="H119" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I119" s="2" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D120" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="E120" s="2">
+        <v>4</v>
+      </c>
+      <c r="F120" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="H120" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I120" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="B122" s="6"/>
+      <c r="C122" s="3"/>
+      <c r="D122" s="3"/>
+      <c r="E122" s="3"/>
+      <c r="F122" s="3"/>
+      <c r="G122" s="3"/>
+      <c r="H122" s="3"/>
+      <c r="I122" s="3"/>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="2">
+        <v>1</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G123" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H123" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="E124" s="2">
+        <v>1</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E125" s="2">
+        <v>1</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H125" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I125" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="E126" s="2">
+        <v>1</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H126" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I126" s="2" t="s">
+        <v>255</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" scale="58" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>